<commit_message>
Alterar números de interface...
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,9 @@
       <c r="I2" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="J2" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,22 +482,25 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="F3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza remaining cost, e solver atualizado
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -501,13 +501,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>3</v>

</xml_diff>